<commit_message>
Done reports, changed encoding to UTF-8, fixed xlsx
</commit_message>
<xml_diff>
--- a/report/lab3.xlsx
+++ b/report/lab3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Inst\3 course\5 sem\par_prog\labs\3\par_prog-3\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79561220-29B8-4728-B653-E72D25C03542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D3AD1-BAD6-455D-8984-DCBA73AD0F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -4173,20 +4173,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="11.47265625" customWidth="1"/>
-    <col min="10" max="10" width="11.62890625" customWidth="1"/>
-    <col min="11" max="12" width="14.578125" customWidth="1"/>
-    <col min="13" max="13" width="15.15625" customWidth="1"/>
-    <col min="14" max="14" width="15.89453125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4262,7 +4263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4300,7 +4301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -4490,7 +4491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -4528,7 +4529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4566,7 +4567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -4642,7 +4643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -4680,7 +4681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -4718,7 +4719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -4756,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -4794,7 +4795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -4832,7 +4833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -4843,7 +4844,7 @@
         <v>7.8165389999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4854,7 +4855,7 @@
         <v>8.2474410000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4865,7 +4866,7 @@
         <v>7.9019180000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -4876,7 +4877,7 @@
         <v>7.9448559999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>5.9457199999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -4898,7 +4899,7 @@
         <v>6.0606350000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -4909,7 +4910,7 @@
         <v>6.3898820000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -4920,7 +4921,7 @@
         <v>6.2999070000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -4931,7 +4932,7 @@
         <v>6.6855880000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -4942,7 +4943,7 @@
         <v>6.4152820000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>5.8853289999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -4964,7 +4965,7 @@
         <v>6.1887610000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -4975,7 +4976,7 @@
         <v>6.104457</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -4986,7 +4987,7 @@
         <v>6.1694290000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -4997,7 +4998,7 @@
         <v>5.3410330000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>5.2276809999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>5.1461480000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -5030,7 +5031,7 @@
         <v>5.1929270000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -5041,7 +5042,7 @@
         <v>5.207541</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>4.9688530000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -5063,7 +5064,7 @@
         <v>5.1823880000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4</v>
       </c>
@@ -5074,7 +5075,7 @@
         <v>5.1629379999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -5085,7 +5086,7 @@
         <v>5.2766500000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -5096,7 +5097,7 @@
         <v>5.1655540000000002</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -5107,7 +5108,7 @@
         <v>4.2726129999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5</v>
       </c>
@@ -5118,7 +5119,7 @@
         <v>4.1385240000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -5129,7 +5130,7 @@
         <v>4.2012429999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
@@ -5140,7 +5141,7 @@
         <v>4.1902999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -5151,7 +5152,7 @@
         <v>4.3363610000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>5</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>4.3829989999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -5173,7 +5174,7 @@
         <v>4.481592</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>5</v>
       </c>
@@ -5184,7 +5185,7 @@
         <v>4.3475760000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>5</v>
       </c>
@@ -5195,7 +5196,7 @@
         <v>4.461684</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>5</v>
       </c>
@@ -5206,7 +5207,7 @@
         <v>4.5159349999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6</v>
       </c>
@@ -5217,7 +5218,7 @@
         <v>3.7343000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>6</v>
       </c>
@@ -5228,7 +5229,7 @@
         <v>3.8905789999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>6</v>
       </c>
@@ -5239,7 +5240,7 @@
         <v>4.0270419999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6</v>
       </c>
@@ -5250,7 +5251,7 @@
         <v>3.840789</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>6</v>
       </c>
@@ -5261,7 +5262,7 @@
         <v>3.832303</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>6</v>
       </c>
@@ -5272,7 +5273,7 @@
         <v>3.844935</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>6</v>
       </c>
@@ -5283,7 +5284,7 @@
         <v>3.8070900000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>6</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>4.045185</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6</v>
       </c>
@@ -5305,7 +5306,7 @@
         <v>3.730553</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -5316,7 +5317,7 @@
         <v>3.9705889999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7</v>
       </c>
@@ -5327,7 +5328,7 @@
         <v>3.6393309999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7</v>
       </c>
@@ -5338,7 +5339,7 @@
         <v>3.475031</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7</v>
       </c>
@@ -5349,7 +5350,7 @@
         <v>3.5903170000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>3.445214</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7</v>
       </c>
@@ -5371,7 +5372,7 @@
         <v>3.505509</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7</v>
       </c>
@@ -5382,7 +5383,7 @@
         <v>3.422523</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7</v>
       </c>
@@ -5393,7 +5394,7 @@
         <v>3.5281020000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7</v>
       </c>
@@ -5404,7 +5405,7 @@
         <v>3.4704959999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>7</v>
       </c>
@@ -5415,7 +5416,7 @@
         <v>3.600962</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7</v>
       </c>
@@ -5426,7 +5427,7 @@
         <v>3.5696680000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>8</v>
       </c>
@@ -5437,7 +5438,7 @@
         <v>3.2857639999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8</v>
       </c>
@@ -5448,7 +5449,7 @@
         <v>3.4056129999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>8</v>
       </c>
@@ -5459,7 +5460,7 @@
         <v>3.2411439999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>8</v>
       </c>
@@ -5470,7 +5471,7 @@
         <v>3.13774</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>8</v>
       </c>
@@ -5481,7 +5482,7 @@
         <v>3.3062429999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>8</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>3.3556469999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8</v>
       </c>
@@ -5503,7 +5504,7 @@
         <v>3.2448630000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>3.1261030000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>8</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>3.2171880000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>8</v>
       </c>
@@ -5536,7 +5537,7 @@
         <v>3.2506979999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9</v>
       </c>
@@ -5547,7 +5548,7 @@
         <v>2.810419</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9</v>
       </c>
@@ -5558,7 +5559,7 @@
         <v>2.875343</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>9</v>
       </c>
@@ -5569,7 +5570,7 @@
         <v>2.9154879999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9</v>
       </c>
@@ -5580,7 +5581,7 @@
         <v>2.9470109999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>2.863318</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9</v>
       </c>
@@ -5602,7 +5603,7 @@
         <v>2.916744</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>9</v>
       </c>
@@ -5613,7 +5614,7 @@
         <v>2.9195540000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9</v>
       </c>
@@ -5624,7 +5625,7 @@
         <v>2.9096799999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9</v>
       </c>
@@ -5635,7 +5636,7 @@
         <v>3.0352420000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9</v>
       </c>
@@ -5646,7 +5647,7 @@
         <v>3.0420750000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>10</v>
       </c>
@@ -5657,7 +5658,7 @@
         <v>2.7134160000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>10</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>2.6709230000000002</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>10</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>2.7666789999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>10</v>
       </c>
@@ -5690,7 +5691,7 @@
         <v>2.6973880000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>10</v>
       </c>
@@ -5701,7 +5702,7 @@
         <v>2.6043859999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>10</v>
       </c>
@@ -5712,7 +5713,7 @@
         <v>2.7793749999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>10</v>
       </c>
@@ -5723,7 +5724,7 @@
         <v>2.7727089999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>10</v>
       </c>
@@ -5734,7 +5735,7 @@
         <v>2.604241</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>10</v>
       </c>
@@ -5745,7 +5746,7 @@
         <v>2.698137</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>10</v>
       </c>
@@ -5756,7 +5757,7 @@
         <v>2.6103269999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>11</v>
       </c>
@@ -5767,7 +5768,7 @@
         <v>2.4458319999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>11</v>
       </c>
@@ -5778,7 +5779,7 @@
         <v>2.5697329999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>11</v>
       </c>
@@ -5789,7 +5790,7 @@
         <v>2.500575</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>11</v>
       </c>
@@ -5800,7 +5801,7 @@
         <v>2.5311889999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>11</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>2.5687690000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>11</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>2.557785</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>11</v>
       </c>
@@ -5833,7 +5834,7 @@
         <v>2.5421320000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>11</v>
       </c>
@@ -5844,7 +5845,7 @@
         <v>2.4716239999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>11</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>2.4788700000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>11</v>
       </c>
@@ -5866,7 +5867,7 @@
         <v>2.5306380000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>12</v>
       </c>
@@ -5877,7 +5878,7 @@
         <v>2.437503</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>12</v>
       </c>
@@ -5888,7 +5889,7 @@
         <v>2.4244599999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>12</v>
       </c>
@@ -5899,7 +5900,7 @@
         <v>2.487015</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>12</v>
       </c>
@@ -5910,7 +5911,7 @@
         <v>2.39269</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>12</v>
       </c>
@@ -5921,7 +5922,7 @@
         <v>2.5045790000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>12</v>
       </c>
@@ -5932,7 +5933,7 @@
         <v>2.4266160000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>12</v>
       </c>
@@ -5943,7 +5944,7 @@
         <v>2.5049429999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>12</v>
       </c>
@@ -5954,7 +5955,7 @@
         <v>2.4802089999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>12</v>
       </c>
@@ -5965,7 +5966,7 @@
         <v>2.3866070000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>12</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>2.4235549999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>13</v>
       </c>
@@ -5987,7 +5988,7 @@
         <v>2.394244</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>13</v>
       </c>
@@ -5998,7 +5999,7 @@
         <v>2.347483</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>13</v>
       </c>
@@ -6009,7 +6010,7 @@
         <v>2.3221090000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>13</v>
       </c>
@@ -6020,7 +6021,7 @@
         <v>2.2578860000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>13</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>2.3513459999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>13</v>
       </c>
@@ -6042,7 +6043,7 @@
         <v>2.3165610000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>13</v>
       </c>
@@ -6053,7 +6054,7 @@
         <v>2.3043390000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>13</v>
       </c>
@@ -6064,7 +6065,7 @@
         <v>2.263001</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>13</v>
       </c>
@@ -6075,7 +6076,7 @@
         <v>2.359823</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>13</v>
       </c>
@@ -6086,7 +6087,7 @@
         <v>2.2883529999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>14</v>
       </c>
@@ -6097,7 +6098,7 @@
         <v>2.251449</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>14</v>
       </c>
@@ -6108,7 +6109,7 @@
         <v>2.345567</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>14</v>
       </c>
@@ -6119,7 +6120,7 @@
         <v>2.2689339999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>14</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>2.286934</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>14</v>
       </c>
@@ -6141,7 +6142,7 @@
         <v>2.2390509999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>14</v>
       </c>
@@ -6152,7 +6153,7 @@
         <v>2.3072629999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>14</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>2.2489720000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>14</v>
       </c>
@@ -6174,7 +6175,7 @@
         <v>2.30158</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>14</v>
       </c>
@@ -6185,7 +6186,7 @@
         <v>2.2234780000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>14</v>
       </c>
@@ -6196,7 +6197,7 @@
         <v>2.2839689999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>15</v>
       </c>
@@ -6207,7 +6208,7 @@
         <v>2.1743619999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>15</v>
       </c>
@@ -6218,7 +6219,7 @@
         <v>2.2260300000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>15</v>
       </c>
@@ -6229,7 +6230,7 @@
         <v>2.2766790000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>15</v>
       </c>
@@ -6240,7 +6241,7 @@
         <v>2.2153870000000002</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>15</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>2.1860040000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>15</v>
       </c>
@@ -6262,7 +6263,7 @@
         <v>2.1354160000000002</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>15</v>
       </c>
@@ -6273,7 +6274,7 @@
         <v>2.2977460000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>15</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>2.2116799999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>15</v>
       </c>
@@ -6295,7 +6296,7 @@
         <v>2.2842479999999998</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>15</v>
       </c>
@@ -6306,7 +6307,7 @@
         <v>2.1865079999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>16</v>
       </c>
@@ -6317,7 +6318,7 @@
         <v>2.1394250000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>16</v>
       </c>
@@ -6328,7 +6329,7 @@
         <v>2.2852800000000002</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>16</v>
       </c>
@@ -6339,7 +6340,7 @@
         <v>2.1988780000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>16</v>
       </c>
@@ -6350,7 +6351,7 @@
         <v>2.0980789999999998</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>16</v>
       </c>
@@ -6361,7 +6362,7 @@
         <v>2.1998099999999998</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>16</v>
       </c>
@@ -6372,7 +6373,7 @@
         <v>2.5318360000000002</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>16</v>
       </c>
@@ -6383,7 +6384,7 @@
         <v>2.196631</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>16</v>
       </c>
@@ -6394,7 +6395,7 @@
         <v>2.1493760000000002</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>16</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>2.159853</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>16</v>
       </c>

</xml_diff>